<commit_message>
fix table grade filling
</commit_message>
<xml_diff>
--- a/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/212/table.xlsx
+++ b/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/212/table.xlsx
@@ -52,7 +52,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,55 +74,11 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="00000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="00000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -130,16 +86,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -519,21 +470,6 @@
           <t>Yandex</t>
         </is>
       </c>
-      <c r="C1" s="7" t="n"/>
-      <c r="D1" s="7" t="n"/>
-      <c r="E1" s="7" t="n"/>
-      <c r="F1" s="7" t="n"/>
-      <c r="G1" s="7" t="n"/>
-      <c r="H1" s="7" t="n"/>
-      <c r="I1" s="7" t="n"/>
-      <c r="J1" s="7" t="n"/>
-      <c r="K1" s="7" t="n"/>
-      <c r="L1" s="7" t="n"/>
-      <c r="M1" s="7" t="n"/>
-      <c r="N1" s="7" t="n"/>
-      <c r="O1" s="7" t="n"/>
-      <c r="P1" s="7" t="n"/>
-      <c r="Q1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -541,24 +477,9 @@
           <t>contest 48711</t>
         </is>
       </c>
-      <c r="C2" s="7" t="n"/>
-      <c r="D2" s="7" t="n"/>
-      <c r="E2" s="7" t="n"/>
-      <c r="F2" s="7" t="n"/>
-      <c r="G2" s="7" t="n"/>
-      <c r="H2" s="7" t="n"/>
-      <c r="I2" s="7" t="n"/>
-      <c r="J2" s="7" t="n"/>
-      <c r="K2" s="7" t="n"/>
-      <c r="L2" s="7" t="n"/>
-      <c r="M2" s="7" t="n"/>
-      <c r="N2" s="7" t="n"/>
-      <c r="O2" s="7" t="n"/>
-      <c r="P2" s="7" t="n"/>
-      <c r="Q2" s="8" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
@@ -638,7 +559,7 @@
           <t>O*</t>
         </is>
       </c>
-      <c r="Q3" s="5" t="inlineStr">
+      <c r="Q3" s="3" t="inlineStr">
         <is>
           <t>Score</t>
         </is>
@@ -650,53 +571,53 @@
           <t>Абабков Даниил</t>
         </is>
       </c>
-      <c r="B4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>0</v>
+      <c r="B4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
@@ -705,53 +626,53 @@
           <t>Гусев Александр Дмитриевич</t>
         </is>
       </c>
-      <c r="B5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="6" t="n">
-        <v>0</v>
+      <c r="B5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="5" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -760,53 +681,53 @@
           <t>hse-compds-2022-46</t>
         </is>
       </c>
-      <c r="B6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="6" t="n">
-        <v>0</v>
+      <c r="B6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="5" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more table formatting + table deletion
</commit_message>
<xml_diff>
--- a/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/212/table.xlsx
+++ b/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/212/table.xlsx
@@ -17,13 +17,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Sans"/>
+      <sz val="20"/>
+    </font>
+    <font>
+      <name val="Sans"/>
+      <sz val="16"/>
     </font>
     <font>
       <name val="Sans"/>
@@ -34,12 +42,8 @@
       <name val="Sans"/>
       <sz val="22"/>
     </font>
-    <font>
-      <name val="Sans"/>
-      <sz val="20"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -51,8 +55,13 @@
         <fgColor rgb="00FFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -74,23 +83,72 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -456,7 +514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +528,26 @@
           <t>Yandex</t>
         </is>
       </c>
+      <c r="C1" s="6" t="n"/>
+      <c r="D1" s="6" t="n"/>
+      <c r="E1" s="6" t="n"/>
+      <c r="F1" s="6" t="n"/>
+      <c r="G1" s="6" t="n"/>
+      <c r="H1" s="6" t="n"/>
+      <c r="I1" s="6" t="n"/>
+      <c r="J1" s="6" t="n"/>
+      <c r="K1" s="6" t="n"/>
+      <c r="L1" s="6" t="n"/>
+      <c r="M1" s="6" t="n"/>
+      <c r="N1" s="6" t="n"/>
+      <c r="O1" s="6" t="n"/>
+      <c r="P1" s="6" t="n"/>
+      <c r="Q1" s="7" t="n"/>
+      <c r="S1" s="8" t="inlineStr">
+        <is>
+          <t>Stepik</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="inlineStr">
@@ -477,6 +555,26 @@
           <t>contest 48711</t>
         </is>
       </c>
+      <c r="C2" s="6" t="n"/>
+      <c r="D2" s="6" t="n"/>
+      <c r="E2" s="6" t="n"/>
+      <c r="F2" s="6" t="n"/>
+      <c r="G2" s="6" t="n"/>
+      <c r="H2" s="6" t="n"/>
+      <c r="I2" s="6" t="n"/>
+      <c r="J2" s="6" t="n"/>
+      <c r="K2" s="6" t="n"/>
+      <c r="L2" s="6" t="n"/>
+      <c r="M2" s="6" t="n"/>
+      <c r="N2" s="6" t="n"/>
+      <c r="O2" s="6" t="n"/>
+      <c r="P2" s="6" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+      <c r="S2" s="2" t="inlineStr">
+        <is>
+          <t>contest 699629</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -564,9 +662,99 @@
           <t>Score</t>
         </is>
       </c>
+      <c r="R3" s="3" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="S3" s="4" t="inlineStr">
+        <is>
+          <t>2903233</t>
+        </is>
+      </c>
+      <c r="T3" s="4" t="inlineStr">
+        <is>
+          <t>2903234</t>
+        </is>
+      </c>
+      <c r="U3" s="4" t="inlineStr">
+        <is>
+          <t>2903237</t>
+        </is>
+      </c>
+      <c r="V3" s="4" t="inlineStr">
+        <is>
+          <t>2903241</t>
+        </is>
+      </c>
+      <c r="W3" s="4" t="inlineStr">
+        <is>
+          <t>2903238</t>
+        </is>
+      </c>
+      <c r="X3" s="4" t="inlineStr">
+        <is>
+          <t>2903239</t>
+        </is>
+      </c>
+      <c r="Y3" s="4" t="inlineStr">
+        <is>
+          <t>2903240</t>
+        </is>
+      </c>
+      <c r="Z3" s="4" t="inlineStr">
+        <is>
+          <t>2903242</t>
+        </is>
+      </c>
+      <c r="AA3" s="4" t="inlineStr">
+        <is>
+          <t>2903401</t>
+        </is>
+      </c>
+      <c r="AB3" s="4" t="inlineStr">
+        <is>
+          <t>2903402</t>
+        </is>
+      </c>
+      <c r="AC3" s="4" t="inlineStr">
+        <is>
+          <t>2903405</t>
+        </is>
+      </c>
+      <c r="AD3" s="4" t="inlineStr">
+        <is>
+          <t>2903404</t>
+        </is>
+      </c>
+      <c r="AE3" s="4" t="inlineStr">
+        <is>
+          <t>2903403</t>
+        </is>
+      </c>
+      <c r="AF3" s="4" t="inlineStr">
+        <is>
+          <t>2903408</t>
+        </is>
+      </c>
+      <c r="AG3" s="4" t="inlineStr">
+        <is>
+          <t>2903406</t>
+        </is>
+      </c>
+      <c r="AH3" s="4" t="inlineStr">
+        <is>
+          <t>2903407</t>
+        </is>
+      </c>
+      <c r="AI3" s="3" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Абабков Даниил</t>
         </is>
@@ -619,9 +807,65 @@
       <c r="Q4" s="5" t="n">
         <v>7</v>
       </c>
+      <c r="R4" s="5" t="inlineStr">
+        <is>
+          <t>Danil Sidorov</t>
+        </is>
+      </c>
+      <c r="S4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="5" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Гусев Александр Дмитриевич</t>
         </is>
@@ -674,9 +918,65 @@
       <c r="Q5" s="5" t="n">
         <v>11</v>
       </c>
+      <c r="R5" s="5" t="inlineStr">
+        <is>
+          <t>Шмаков Валерий</t>
+        </is>
+      </c>
+      <c r="S5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="5" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>hse-compds-2022-46</t>
         </is>
@@ -729,10 +1029,126 @@
       <c r="Q6" s="5" t="n">
         <v>5</v>
       </c>
+      <c r="R6" s="5" t="inlineStr">
+        <is>
+          <t>Юрий Донской</t>
+        </is>
+      </c>
+      <c r="S6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="5" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="R7" s="5" t="inlineStr">
+        <is>
+          <t>кленин</t>
+        </is>
+      </c>
+      <c r="S7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="5" t="n">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="S2:AI2"/>
+    <mergeCell ref="S1:AI1"/>
     <mergeCell ref="B1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>